<commit_message>
Add employee and supervisor data loading, implement sales upload functionality, and create processes HTML template
- Implemented loading of employee and supervisor data from APIs in dashboard.js.
- Added file upload functionality for sales data in procesos.js.
- Created a new HTML template for processes with sidebar navigation and file upload button.
- Updated static assets including images and styles for the new processes page.
</commit_message>
<xml_diff>
--- a/Plantillas Carga Datos/Plantilla Objetivos.xlsx
+++ b/Plantillas Carga Datos/Plantilla Objetivos.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\HeroApp #2\MyPage\Plantillas Carga Datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2C2FD1C-D21B-489C-AF34-7865059CF5F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F23F5D80-3D53-4772-96B4-DB24DEF1DBF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -113,7 +113,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -124,6 +124,12 @@
       <patternFill patternType="solid">
         <fgColor indexed="20"/>
         <bgColor indexed="24"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -154,7 +160,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -167,6 +173,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -449,10 +458,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N42"/>
+  <dimension ref="A1:N43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="C53" sqref="C53"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="N44" sqref="N44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="47.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -522,13 +531,13 @@
         <v>1013436</v>
       </c>
       <c r="B2" s="4">
-        <v>45931</v>
+        <v>45962</v>
       </c>
       <c r="C2" s="3">
         <v>35</v>
       </c>
       <c r="D2" s="3">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E2" s="3">
         <v>1</v>
@@ -566,7 +575,7 @@
         <v>1004203</v>
       </c>
       <c r="B3" s="4">
-        <v>45931</v>
+        <v>45962</v>
       </c>
       <c r="C3" s="3">
         <v>40</v>
@@ -610,7 +619,7 @@
         <v>1025809</v>
       </c>
       <c r="B4" s="4">
-        <v>45931</v>
+        <v>45962</v>
       </c>
       <c r="C4" s="3">
         <v>30</v>
@@ -654,7 +663,7 @@
         <v>1026182</v>
       </c>
       <c r="B5" s="4">
-        <v>45931</v>
+        <v>45962</v>
       </c>
       <c r="C5" s="3">
         <v>40</v>
@@ -698,7 +707,7 @@
         <v>1026181</v>
       </c>
       <c r="B6" s="4">
-        <v>45931</v>
+        <v>45962</v>
       </c>
       <c r="C6" s="3">
         <v>40</v>
@@ -742,7 +751,7 @@
         <v>1015360</v>
       </c>
       <c r="B7" s="4">
-        <v>45931</v>
+        <v>45962</v>
       </c>
       <c r="C7" s="3">
         <v>40</v>
@@ -786,7 +795,7 @@
         <v>1020523</v>
       </c>
       <c r="B8" s="4">
-        <v>45931</v>
+        <v>45962</v>
       </c>
       <c r="C8" s="3">
         <v>40</v>
@@ -830,40 +839,40 @@
         <v>1014158</v>
       </c>
       <c r="B9" s="4">
-        <v>45931</v>
+        <v>45962</v>
       </c>
       <c r="C9" s="3">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="D9" s="3">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="E9" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F9" s="3">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G9" s="3">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H9" s="3">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I9" s="3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J9" s="3">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="K9" s="3">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="L9" s="3">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="M9" s="3">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="N9" s="3">
         <v>9000</v>
@@ -874,7 +883,7 @@
         <v>1015856</v>
       </c>
       <c r="B10" s="4">
-        <v>45931</v>
+        <v>45962</v>
       </c>
       <c r="C10" s="3">
         <v>40</v>
@@ -901,7 +910,7 @@
         <v>4</v>
       </c>
       <c r="K10" s="3">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="L10" s="3">
         <v>2</v>
@@ -918,7 +927,7 @@
         <v>1004198</v>
       </c>
       <c r="B11" s="4">
-        <v>45931</v>
+        <v>45962</v>
       </c>
       <c r="C11" s="3">
         <v>45</v>
@@ -962,13 +971,13 @@
         <v>1026014</v>
       </c>
       <c r="B12" s="4">
-        <v>45931</v>
+        <v>45962</v>
       </c>
       <c r="C12" s="3">
         <v>30</v>
       </c>
       <c r="D12" s="3">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E12" s="3">
         <v>1</v>
@@ -989,7 +998,7 @@
         <v>2</v>
       </c>
       <c r="K12" s="3">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="L12" s="3">
         <v>2</v>
@@ -1006,13 +1015,13 @@
         <v>1016723</v>
       </c>
       <c r="B13" s="4">
-        <v>45931</v>
+        <v>45962</v>
       </c>
       <c r="C13" s="3">
         <v>40</v>
       </c>
       <c r="D13" s="3">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E13" s="3">
         <v>1</v>
@@ -1033,7 +1042,7 @@
         <v>4</v>
       </c>
       <c r="K13" s="3">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="L13" s="3">
         <v>3</v>
@@ -1050,43 +1059,43 @@
         <v>1023030</v>
       </c>
       <c r="B14" s="4">
-        <v>45931</v>
+        <v>45962</v>
       </c>
       <c r="C14" s="3">
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="D14" s="3">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="E14" s="3">
         <v>1</v>
       </c>
       <c r="F14" s="3">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G14" s="3">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="H14" s="3">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="I14" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J14" s="3">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="K14" s="3">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="L14" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="M14" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="N14" s="3">
-        <v>9000</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
@@ -1094,7 +1103,7 @@
         <v>1020590</v>
       </c>
       <c r="B15" s="4">
-        <v>45931</v>
+        <v>45962</v>
       </c>
       <c r="C15" s="3">
         <v>35</v>
@@ -1138,7 +1147,7 @@
         <v>1020293</v>
       </c>
       <c r="B16" s="4">
-        <v>45931</v>
+        <v>45962</v>
       </c>
       <c r="C16" s="3">
         <v>40</v>
@@ -1182,7 +1191,7 @@
         <v>1018461</v>
       </c>
       <c r="B17" s="4">
-        <v>45931</v>
+        <v>45962</v>
       </c>
       <c r="C17" s="3">
         <v>35</v>
@@ -1226,7 +1235,7 @@
         <v>1008649</v>
       </c>
       <c r="B18" s="4">
-        <v>45931</v>
+        <v>45962</v>
       </c>
       <c r="C18" s="3">
         <v>40</v>
@@ -1270,7 +1279,7 @@
         <v>1020591</v>
       </c>
       <c r="B19" s="4">
-        <v>45931</v>
+        <v>45962</v>
       </c>
       <c r="C19" s="3">
         <v>40</v>
@@ -1314,7 +1323,7 @@
         <v>1014718</v>
       </c>
       <c r="B20" s="4">
-        <v>45931</v>
+        <v>45962</v>
       </c>
       <c r="C20" s="3">
         <v>40</v>
@@ -1358,7 +1367,7 @@
         <v>1018939</v>
       </c>
       <c r="B21" s="4">
-        <v>45931</v>
+        <v>45962</v>
       </c>
       <c r="C21" s="3">
         <v>60</v>
@@ -1402,7 +1411,7 @@
         <v>1019285</v>
       </c>
       <c r="B22" s="4">
-        <v>45931</v>
+        <v>45962</v>
       </c>
       <c r="C22" s="3">
         <v>35</v>
@@ -1446,7 +1455,7 @@
         <v>1023692</v>
       </c>
       <c r="B23" s="4">
-        <v>45931</v>
+        <v>45962</v>
       </c>
       <c r="C23" s="3">
         <v>60</v>
@@ -1490,7 +1499,7 @@
         <v>1010668</v>
       </c>
       <c r="B24" s="4">
-        <v>45931</v>
+        <v>45962</v>
       </c>
       <c r="C24" s="3">
         <v>30</v>
@@ -1534,7 +1543,7 @@
         <v>1013841</v>
       </c>
       <c r="B25" s="4">
-        <v>45931</v>
+        <v>45962</v>
       </c>
       <c r="C25" s="3">
         <v>25</v>
@@ -1578,7 +1587,7 @@
         <v>1010053</v>
       </c>
       <c r="B26" s="4">
-        <v>45931</v>
+        <v>45962</v>
       </c>
       <c r="C26" s="3">
         <v>45</v>
@@ -1622,7 +1631,7 @@
         <v>1026198</v>
       </c>
       <c r="B27" s="4">
-        <v>45931</v>
+        <v>45962</v>
       </c>
       <c r="C27" s="3">
         <v>40</v>
@@ -1666,7 +1675,7 @@
         <v>1025681</v>
       </c>
       <c r="B28" s="4">
-        <v>45931</v>
+        <v>45962</v>
       </c>
       <c r="C28" s="3">
         <v>40</v>
@@ -1710,7 +1719,7 @@
         <v>1008917</v>
       </c>
       <c r="B29" s="4">
-        <v>45931</v>
+        <v>45962</v>
       </c>
       <c r="C29" s="3">
         <v>40</v>
@@ -1754,7 +1763,7 @@
         <v>1025570</v>
       </c>
       <c r="B30" s="4">
-        <v>45931</v>
+        <v>45962</v>
       </c>
       <c r="C30" s="3">
         <v>25</v>
@@ -1798,7 +1807,7 @@
         <v>1025959</v>
       </c>
       <c r="B31" s="4">
-        <v>45931</v>
+        <v>45962</v>
       </c>
       <c r="C31" s="3">
         <v>30</v>
@@ -1842,7 +1851,7 @@
         <v>1014788</v>
       </c>
       <c r="B32" s="4">
-        <v>45931</v>
+        <v>45962</v>
       </c>
       <c r="C32" s="3">
         <v>40</v>
@@ -1886,7 +1895,7 @@
         <v>1023505</v>
       </c>
       <c r="B33" s="4">
-        <v>45931</v>
+        <v>45962</v>
       </c>
       <c r="C33" s="3">
         <v>30</v>
@@ -1930,7 +1939,7 @@
         <v>1025411</v>
       </c>
       <c r="B34" s="4">
-        <v>45931</v>
+        <v>45962</v>
       </c>
       <c r="C34" s="3">
         <v>35</v>
@@ -1974,7 +1983,7 @@
         <v>1023651</v>
       </c>
       <c r="B35" s="4">
-        <v>45931</v>
+        <v>45962</v>
       </c>
       <c r="C35" s="3">
         <v>1</v>
@@ -2018,7 +2027,7 @@
         <v>1017156</v>
       </c>
       <c r="B36" s="4">
-        <v>45931</v>
+        <v>45962</v>
       </c>
       <c r="C36" s="3">
         <v>35</v>
@@ -2062,7 +2071,7 @@
         <v>1004208</v>
       </c>
       <c r="B37" s="4">
-        <v>45931</v>
+        <v>45962</v>
       </c>
       <c r="C37" s="3">
         <v>35</v>
@@ -2106,7 +2115,7 @@
         <v>1018541</v>
       </c>
       <c r="B38" s="4">
-        <v>45931</v>
+        <v>45962</v>
       </c>
       <c r="C38" s="3">
         <v>35</v>
@@ -2150,7 +2159,7 @@
         <v>1025454</v>
       </c>
       <c r="B39" s="4">
-        <v>45931</v>
+        <v>45962</v>
       </c>
       <c r="C39" s="3">
         <v>60</v>
@@ -2194,7 +2203,7 @@
         <v>1020719</v>
       </c>
       <c r="B40" s="4">
-        <v>45931</v>
+        <v>45962</v>
       </c>
       <c r="C40" s="3">
         <v>35</v>
@@ -2238,7 +2247,7 @@
         <v>1012502</v>
       </c>
       <c r="B41" s="4">
-        <v>45931</v>
+        <v>45962</v>
       </c>
       <c r="C41" s="3">
         <v>25</v>
@@ -2278,10 +2287,12 @@
       </c>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A42" s="2">
+      <c r="A42" s="6">
         <v>1025113</v>
       </c>
-      <c r="B42" s="4"/>
+      <c r="B42" s="4">
+        <v>45962</v>
+      </c>
       <c r="C42" s="3">
         <v>1</v>
       </c>
@@ -2316,7 +2327,51 @@
         <v>1</v>
       </c>
       <c r="N42" s="3">
-        <v>9000</v>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A43" s="6">
+        <v>1017255</v>
+      </c>
+      <c r="B43" s="4">
+        <v>45962</v>
+      </c>
+      <c r="C43" s="3">
+        <v>1</v>
+      </c>
+      <c r="D43" s="3">
+        <v>1</v>
+      </c>
+      <c r="E43" s="3">
+        <v>1</v>
+      </c>
+      <c r="F43" s="3">
+        <v>1</v>
+      </c>
+      <c r="G43" s="3">
+        <v>1</v>
+      </c>
+      <c r="H43" s="3">
+        <v>1</v>
+      </c>
+      <c r="I43" s="3">
+        <v>1</v>
+      </c>
+      <c r="J43" s="3">
+        <v>1</v>
+      </c>
+      <c r="K43" s="3">
+        <v>1</v>
+      </c>
+      <c r="L43" s="3">
+        <v>1</v>
+      </c>
+      <c r="M43" s="3">
+        <v>1</v>
+      </c>
+      <c r="N43" s="3">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>